<commit_message>
ticket 165: ajuste en autoadmin para que el campo descriptivo de la clave foranea lo intente tomar primero desde el catalogo, primer campo de plantilla
</commit_message>
<xml_diff>
--- a/public/uploads/${ID_ORDEN_SERVICIO} Orden ${ID_ORDEN_SERVICIO_LETRAS} DATOS ${CONCENTRADOR_CIU_NOMBRE} ${EXTREMO_CIU_NOMBRE}.xlsx
+++ b/public/uploads/${ID_ORDEN_SERVICIO} Orden ${ID_ORDEN_SERVICIO_LETRAS} DATOS ${CONCENTRADOR_CIU_NOMBRE} ${EXTREMO_CIU_NOMBRE}.xlsx
@@ -57,7 +57,7 @@
     <t xml:space="preserve">${CONCENTRADOR_UBI_LATITUD}</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION} ${CONCENTRADOR_LOGIN}</t>
+    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION}</t>
   </si>
   <si>
     <t xml:space="preserve">Punto B</t>
@@ -75,7 +75,7 @@
     <t xml:space="preserve">${EXTREMO_UBI_LATITUD}</t>
   </si>
   <si>
-    <t xml:space="preserve">${EXTREMO_UBI_DIRECCION} ${EXTREMO_LOGIN}</t>
+    <t xml:space="preserve">${EXTREMO_UBI_DIRECCION}</t>
   </si>
 </sst>
 </file>

</xml_diff>